<commit_message>
Updated 835 converter files examples
</commit_message>
<xml_diff>
--- a/converted_files/835/835-all-fields.xlsx
+++ b/converted_files/835/835-all-fields.xlsx
@@ -1110,7 +1110,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -1188,25 +1188,25 @@
       </c>
       <c r="S2" s="3" t="inlineStr">
         <is>
-          <t>CHECK</t>
+          <t>ACH</t>
         </is>
       </c>
       <c r="T2" s="3" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>2200008888</t>
         </is>
       </c>
       <c r="U2" s="4" t="n">
-        <v>43555.0</v>
+        <v>45756.0</v>
       </c>
       <c r="V2" s="3" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>882509401093167</t>
         </is>
       </c>
       <c r="W2" s="3" t="inlineStr">
         <is>
-          <t>1512345678</t>
+          <t>106609999</t>
         </is>
       </c>
       <c r="X2" s="4" t="n">
@@ -1267,8 +1267,16 @@
       <c r="AQ2"/>
       <c r="AR2"/>
       <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>PAYOR_ID</t>
+        </is>
+      </c>
+      <c r="AU2" s="3" t="inlineStr">
+        <is>
+          <t>0101</t>
+        </is>
+      </c>
       <c r="AV2" s="3" t="inlineStr">
         <is>
           <t>DELTA DENTAL OF ABC</t>
@@ -1485,8 +1493,16 @@
           <t>12345678</t>
         </is>
       </c>
-      <c r="CZ2"/>
-      <c r="DA2"/>
+      <c r="CZ2" s="3" t="inlineStr">
+        <is>
+          <t>PROVIDER_UPIN_NUMBER</t>
+        </is>
+      </c>
+      <c r="DA2" s="3" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
       <c r="DB2" s="3" t="inlineStr">
         <is>
           <t>CMS_PLAN_ID</t>
@@ -1796,7 +1812,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B3"/>
@@ -2060,7 +2076,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B4"/>
@@ -2324,7 +2340,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B5"/>
@@ -2588,7 +2604,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B6"/>
@@ -2836,7 +2852,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B7"/>
@@ -3130,7 +3146,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>685d698cd8be1604d3e9fd27</t>
+          <t>68ec56cbce2f64368d177df2</t>
         </is>
       </c>
       <c r="B8"/>

</xml_diff>

<commit_message>
Updated output examples and OpenAPI schemas to include new fields and enums; release 2.14.7
</commit_message>
<xml_diff>
--- a/converted_files/835/835-all-fields.xlsx
+++ b/converted_files/835/835-all-fields.xlsx
@@ -1110,7 +1110,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B3"/>
@@ -2076,7 +2076,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B4"/>
@@ -2340,7 +2340,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B5"/>
@@ -2604,7 +2604,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B6"/>
@@ -2852,7 +2852,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B7"/>
@@ -3146,7 +3146,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>69014027ca84f491f7f21495</t>
+          <t>69446374c1a6b3ab024f4f3b</t>
         </is>
       </c>
       <c r="B8"/>

</xml_diff>